<commit_message>
Add all columns from corpus
</commit_message>
<xml_diff>
--- a/tests/corpus.xlsx
+++ b/tests/corpus.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t xml:space="preserve">Miniature</t>
   </si>
@@ -31,16 +31,52 @@
     <t xml:space="preserve">Auteur</t>
   </si>
   <si>
+    <t xml:space="preserve">Profession</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pays</t>
   </si>
   <si>
+    <t xml:space="preserve">Titre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Publication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thème(s) critique(s) (idées primaires)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paradigme esthétique (idées primaires)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Motifs esthétiques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Registre(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interprétation</t>
+  </si>
+  <si>
     <t xml:space="preserve">John</t>
   </si>
   <si>
+    <t xml:space="preserve">Blabla</t>
+  </si>
+  <si>
     <t xml:space="preserve">Australie</t>
   </si>
   <si>
     <t xml:space="preserve">Albert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boublou</t>
   </si>
   <si>
     <t xml:space="preserve">France</t>
@@ -241,17 +277,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="bottomLeft" activeCell="N2" activeCellId="0" sqref="N2:N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="94.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -263,6 +299,36 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,10 +336,40 @@
         <v>2015</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -281,10 +377,40 @@
         <v>2015</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>17</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>